<commit_message>
Added post req and updated assertions in Spock
</commit_message>
<xml_diff>
--- a/RestApi/data/TestData.xlsx
+++ b/RestApi/data/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Request</t>
   </si>
@@ -31,6 +31,18 @@
   </si>
   <si>
     <t>https://reqres.in/</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>{
+    "name": "RestTest",
+    "job": "Org"
+}</t>
   </si>
 </sst>
 </file>
@@ -95,10 +107,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,19 +418,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -422,8 +441,11 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -433,11 +455,21 @@
       <c r="C2" s="1">
         <v>200</v>
       </c>
+      <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>201</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Bearer token authentication Added Logger
</commit_message>
<xml_diff>
--- a/RestApi/data/TestData.xlsx
+++ b/RestApi/data/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Request</t>
   </si>
@@ -30,19 +30,10 @@
     <t>StatusCode</t>
   </si>
   <si>
-    <t>https://reqres.in/</t>
-  </si>
-  <si>
     <t>Post</t>
   </si>
   <si>
-    <t>Body</t>
-  </si>
-  <si>
-    <t>{
-    "name": "RestTest",
-    "job": "Org"
-}</t>
+    <t>https://bookstore.toolsqa.com</t>
   </si>
 </sst>
 </file>
@@ -115,7 +106,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -418,20 +409,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -441,34 +431,27 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>200</v>
       </c>
-      <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="C3" s="1">
         <v>201</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Put request with bearer authentication
</commit_message>
<xml_diff>
--- a/RestApi/data/TestData.xlsx
+++ b/RestApi/data/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Request</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>https://bookstore.toolsqa.com</t>
+  </si>
+  <si>
+    <t>Put</t>
   </si>
 </sst>
 </file>
@@ -409,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,6 +457,17 @@
         <v>201</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added delete Request and assertions included for same
</commit_message>
<xml_diff>
--- a/RestApi/data/TestData.xlsx
+++ b/RestApi/data/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Request</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Put</t>
+  </si>
+  <si>
+    <t>Delete</t>
   </si>
 </sst>
 </file>
@@ -101,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -111,6 +114,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,6 +472,17 @@
         <v>200</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5">
+        <v>204</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>